<commit_message>
fix: correcao da insercao para segurança, propriedades e atualizaçao final das tabelas
</commit_message>
<xml_diff>
--- a/src/main/resources/files/districts.xlsx
+++ b/src/main/resources/files/districts.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/netoremelli/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC281F3B-ABD9-504C-8002-87F184269F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3520ABC4-97B5-3C4A-B4F1-3D6445A3095B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="2760" windowWidth="26640" windowHeight="15140" xr2:uid="{D51873B7-A091-5D4A-9A4F-56E6D44953A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
-    <t>VILA MARIAN</t>
-  </si>
-  <si>
     <t xml:space="preserve">Distrito               </t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t xml:space="preserve">VILA SONIA </t>
+  </si>
+  <si>
+    <t>VILA MARIANA</t>
   </si>
 </sst>
 </file>
@@ -701,10 +701,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567F9104-819A-6C4A-B2B3-7BA5B21804E4}">
+  <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:B97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,15 +715,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>3550308001</v>
@@ -730,7 +731,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>3550308002</v>
@@ -738,7 +739,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3550308003</v>
@@ -746,7 +747,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>3550308004</v>
@@ -754,7 +755,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>3550308005</v>
@@ -762,7 +763,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>3550308006</v>
@@ -770,7 +771,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>3550308007</v>
@@ -778,7 +779,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>3550308008</v>
@@ -786,7 +787,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>3550308009</v>
@@ -794,7 +795,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>3550308010</v>
@@ -802,7 +803,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>3550308011</v>
@@ -810,7 +811,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>3550308012</v>
@@ -818,7 +819,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>3550308013</v>
@@ -826,7 +827,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>3550308014</v>
@@ -834,7 +835,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>3550308015</v>
@@ -842,7 +843,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>3550308016</v>
@@ -850,7 +851,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>3550308017</v>
@@ -858,7 +859,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>3550308018</v>
@@ -866,7 +867,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>3550308019</v>
@@ -874,7 +875,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>3550308020</v>
@@ -882,7 +883,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>3550308021</v>
@@ -890,7 +891,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>3550308022</v>
@@ -898,7 +899,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>3550308023</v>
@@ -906,7 +907,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>3550308024</v>
@@ -914,7 +915,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>3550308025</v>
@@ -922,7 +923,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>3550308026</v>
@@ -930,7 +931,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>3550308027</v>
@@ -938,7 +939,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>3550308028</v>
@@ -946,7 +947,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>3550308029</v>
@@ -954,7 +955,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>3550308030</v>
@@ -962,7 +963,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>3550308031</v>
@@ -970,7 +971,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>3550308032</v>
@@ -978,7 +979,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>3550308033</v>
@@ -986,7 +987,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>3550308034</v>
@@ -994,7 +995,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36">
         <v>3550308035</v>
@@ -1002,7 +1003,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37">
         <v>3550308036</v>
@@ -1010,7 +1011,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38">
         <v>3550308037</v>
@@ -1018,7 +1019,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39">
         <v>3550308038</v>
@@ -1026,7 +1027,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <v>3550308039</v>
@@ -1034,7 +1035,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41">
         <v>3550308040</v>
@@ -1042,7 +1043,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>3550308041</v>
@@ -1050,7 +1051,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>3550308042</v>
@@ -1058,7 +1059,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>3550308043</v>
@@ -1066,7 +1067,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>3550308044</v>
@@ -1074,7 +1075,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <v>3550308045</v>
@@ -1082,7 +1083,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>3550308046</v>
@@ -1090,7 +1091,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>3550308047</v>
@@ -1098,7 +1099,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>3550308048</v>
@@ -1106,7 +1107,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>3550308049</v>
@@ -1114,7 +1115,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>3550308050</v>
@@ -1122,7 +1123,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52">
         <v>3550308051</v>
@@ -1130,7 +1131,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>3550308052</v>
@@ -1138,7 +1139,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>3550308053</v>
@@ -1146,7 +1147,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>3550308054</v>
@@ -1154,7 +1155,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56">
         <v>3550308055</v>
@@ -1162,7 +1163,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57">
         <v>3550308056</v>
@@ -1170,7 +1171,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58">
         <v>3550308057</v>
@@ -1178,7 +1179,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>3550308058</v>
@@ -1186,7 +1187,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60">
         <v>3550308059</v>
@@ -1194,7 +1195,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61">
         <v>3550308060</v>
@@ -1202,7 +1203,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62">
         <v>3550308061</v>
@@ -1210,7 +1211,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63">
         <v>3550308062</v>
@@ -1218,7 +1219,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64">
         <v>3550308063</v>
@@ -1226,7 +1227,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65">
         <v>3550308064</v>
@@ -1234,7 +1235,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66">
         <v>3550308065</v>
@@ -1242,7 +1243,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67">
         <v>3550308066</v>
@@ -1250,7 +1251,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68">
         <v>3550308067</v>
@@ -1258,7 +1259,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69">
         <v>3550308068</v>
@@ -1266,7 +1267,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70">
         <v>3550308069</v>
@@ -1274,7 +1275,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71">
         <v>3550308070</v>
@@ -1282,7 +1283,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72">
         <v>3550308071</v>
@@ -1290,7 +1291,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73">
         <v>3550308072</v>
@@ -1298,7 +1299,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74">
         <v>3550308073</v>
@@ -1306,7 +1307,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75">
         <v>3550308074</v>
@@ -1314,7 +1315,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76">
         <v>3550308075</v>
@@ -1322,7 +1323,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77">
         <v>3550308076</v>
@@ -1330,7 +1331,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78">
         <v>3550308077</v>
@@ -1338,7 +1339,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B79">
         <v>3550308078</v>
@@ -1346,7 +1347,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B80">
         <v>3550308079</v>
@@ -1354,7 +1355,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81">
         <v>3550308080</v>
@@ -1362,7 +1363,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82">
         <v>3550308081</v>
@@ -1370,7 +1371,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B83">
         <v>3550308082</v>
@@ -1378,7 +1379,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B84">
         <v>3550308083</v>
@@ -1386,7 +1387,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85">
         <v>3550308084</v>
@@ -1394,7 +1395,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86">
         <v>3550308085</v>
@@ -1402,7 +1403,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87">
         <v>3550308086</v>
@@ -1410,7 +1411,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B88">
         <v>3550308087</v>
@@ -1418,7 +1419,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89">
         <v>3550308088</v>
@@ -1426,7 +1427,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90">
         <v>3550308089</v>
@@ -1434,7 +1435,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91">
         <v>3550308090</v>
@@ -1442,7 +1443,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92">
         <v>3550308091</v>
@@ -1450,7 +1451,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B93">
         <v>3550308092</v>
@@ -1458,7 +1459,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94">
         <v>3550308093</v>
@@ -1466,7 +1467,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95">
         <v>3550308094</v>
@@ -1474,7 +1475,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96">
         <v>3550308095</v>
@@ -1482,7 +1483,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97">
         <v>3550308096</v>

</xml_diff>

<commit_message>
fix: correcao da insercao para distrito
</commit_message>
<xml_diff>
--- a/src/main/resources/files/districts.xlsx
+++ b/src/main/resources/files/districts.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/netoremelli/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3520ABC4-97B5-3C4A-B4F1-3D6445A3095B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5914B18-229C-0240-B491-5DCD4B1B92EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="2760" windowWidth="26640" windowHeight="15140" xr2:uid="{D51873B7-A091-5D4A-9A4F-56E6D44953A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$D$97</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="250">
   <si>
     <t xml:space="preserve">Distrito               </t>
   </si>
@@ -330,6 +333,2000 @@
   </si>
   <si>
     <t>VILA MARIANA</t>
+  </si>
+  <si>
+    <t>Area km2</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>bairros associados</t>
+  </si>
+  <si>
+    <t>Jardim Itália
+Jardim Silveira (parte)
+Parque Sevilha
+Vila Bertioga
+Vila Canero
+Vila Celeste
+Vila Cláudia
+Vila Clotilde
+Vila Diva
+Vila Graciosa
+Vila Invernada
+Vila Leme
+Vila Libanesa
+Vila Lúcia Elvira
+Vila Oratório
+Vila Paulina  Chácara Mafalda
+Chácara Paraíso
+Jardim Guanabara
+Vila Regente Feijó
+Vila Rio Branco
+Vila Santa Clara</t>
+  </si>
+  <si>
+    <t>7.7</t>
+  </si>
+  <si>
+    <t>Alto de Pinheiros
+Boaçava
+Jardim Atibaia
+Jardim Califórnia
+Jardim dos Jacarandás
+Jardim Ligia
+Sítio Boa Vista
+Vila Beatriz
+Vila Ida
+Vila Jataí
+Vila Nogueira</t>
+  </si>
+  <si>
+    <t>33.3</t>
+  </si>
+  <si>
+    <t>Chácara Maria Trindade
+Filhos da Terra
+Itaberaba I
+Itaberaba II
+Jardim Anhanguera
+Jardim Boa Vista
+Jardim Britânia
+Jardim Canaã
+Jardim Clei
+Jardim Escócia
+Jardim Jaraguá
+Jardim Monte Belo
+Jardim Palmares
+Jardim Primavera
+Jardim Rosinha
+Jardim Santa Fé
+Morada do Sol
+Morada do Sol (Ao lado do Sol Nascente)
+Parque Morro Doce
+Parque Anhanguera
+Parque Esperança
+Residencial Sol Nascente
+Vila Sulina</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>Aricanduva
+Jardim Antonieta
+Jardim Aricanduva
+Jardim Caguassu
+Jardim Catarina
+Jardim Cotching
+Jardim Galli
+Jardim Guannam
+Jardim Haia do Carrão
+Jardim Iva
+Jardim Machado
+Jardim Nova Carrão
+Jardim Piquerobi
+Jardim Record
+Jardim das Rosas
+Jardim Santo Eduardo
+Jardim Tango
+Jardim Vila Formosa
+Parque Maria Luiza
+Parque Santo Antônio
+Vila Alzira
+Vila Antonieta
+Vila Embira
+Vila Falconi
+Vila Nova Iorque
+Vila Nice
+Vila Rica
+Vila Sara</t>
+  </si>
+  <si>
+    <t>Jardim Marina; Vila Nhocuné; Jardim Cardoso; Jardim São José; Parque Bela Vista; Vila Santa Tereza; Conjunto Habitacional Pe. José de Anchieta; Conjunto Habitacional Pe. Manoel da Nóbrega; Parque Artur Alvim; Cidade A.E. Carvalho (parte); Parque das Paineiras; Conj. Hab. Jardim Marcial; Jardim Nordeste; Jardim Artur Alvim; Jardim Olímpia; Jardim Coimbra; Jardim Brasil; Vila Campanela; Jardim São Nicolau</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>Água Branca
+Barra Funda (parte)
+Vila Barra Funda
+Vila Chalot
+Vila Charlote
+Vila dos Ferroviários
+Parque Industrial Tomas Edson</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>Bela Vista, Morro dos Ingleses, Cerqueira Cesar, Bixiga</t>
+  </si>
+  <si>
+    <t>Belenzinho
+Catumbi
+Chácara Tatuapé
+Quarta Parada
+Vila Maria Zélia</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Brasilândia, Jardim Maracanã; Parque Hollywood; Parque Itaberaba; Jardim Magali; Jardim Elísio; Jardim Alvorada; Jardim Almanara; Vila Elias Nigri; Jardim Irene; Vila Rica; Vila Penteado; Parque Pedroso; Vila Souza; Jardim Ondina; Jardim Ana Maria; Vila Ismênia; Parque Belém; Jardim Elisa Maria; Parque Tietê; Jardim Ladeira Rosa; Vila Terezinha; Vila Dulcina; Vila Isabel; Vila Áurea; Vila Nina; Jardim dos Guedes; Vila Serralheiro; Jardim do Tiro; Vila Itaberaba; Vila Icaraí; Vila São João Batista; Vila São Joaquim; Jardim Paulistano; Jardim Carombé; Jardim Guarani; Jardim Princesa; Jardim Damasceno; Jardim Paraná; Jardim Vista Alegre; Jardim Recanto; Jardim dos Francos</t>
+  </si>
+  <si>
+    <t>12.9</t>
+  </si>
+  <si>
+    <t>City Butantã; Vila Indiana; Jardim Rizzo; Vila Pirajussara; Conjunto Residencial Butantã; Jardim Christi; Jardim Ademar; Previdência; Caxingui; Rolinópolis; Jardim Esmeralda; Vila Gomes; Jardim Bonfiglioli; Jardim São Gilberto; Cidade dos Bandeirantes; Jardim Matarazzo; Jardim Pinheiros.</t>
+  </si>
+  <si>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>Vila Nova Cachoeirinha; Vila Cachoeirinha; Vila P Rosa Branca; Vila dos Andrades; Vila Celeste; Vila Paulo Raveli; Vila Roque; Vila Rita; Jardim Nossa Sra. da Consolata; Jardim Imirim; Vila Amélia; Sítio Casa Verde; CPO. da Água Branca; Jardim Centenário; Vila Angélica; Vila Dionísia; Vila Continental; Vila Amália; Vila Bela Vista: Jardim Ceci; Jardim Santa Cruz; Jardim Peri; Jardim Peri Novo; Jardim Antártica.</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>Brooklin Velho
+Campo Belo
+Jardim Aeroporto
+Jardim Brasil
+Jardim Rutinha
+Vila Aeroporto
+Vila Alexandrina
+Vila Canaã
+Vila Carmem
+Vila Congonhas
+Parque Jabaquara</t>
+  </si>
+  <si>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>12.6</t>
+  </si>
+  <si>
+    <t>ardim Jaú (Parte); Vila Londrina; Vila Mesquita; Vila Santo Henrique; Jardim Otília; Vila Paz; Jardim Gôndolo; Vila Dom Duarte Leopoldo; Jardim de Lorenzo; Chácara Cruz do Sul; Vila Pierina; Vila Vidal; Vila Rui Barbosa; Vila Araguaia; Vila Penteado; Chácara Santo Antônio; Jardim Arizona; Jardim Cangaíba; Jardim Piratininga; Vila Fernando; Vila Rufino; Jardim Paulistânia; Vila Hilda; Vila Antenor; Vila Rica; Jardim São Francisco; Vila Arruda; Vila Sartori; Jardim Janiópolis; Engenheiro Goulart; Vila Brasil; Vila Buenos Aires; Jardim do Castelo; Vila Franci; Vila Belo Horizonte; Vila Libanesa; Parque Líbano; Vila Sílvia; Jardim Danfer; Vila Amália; Jardim Gonzaga; Vila São Jorge; Jardim Penha; Jardim Aidar; Vila Guaraciaba (Parte)</t>
+  </si>
+  <si>
+    <t>13.8</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>Chácara Califórnia
+Chácara Santo Antônio
+Vila Carrão
+Vila Nova Manchester
+Vila Santa Isabel
+Jardim Têxtil (parte)
+Vila Santo Estevão
+Carrãozinho</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Casa Verde; Casa Verde Baixa; Casa Verde Média; Casa Verde Alta; Vila Baruel; Parque Souza Aranha; Jardim das Laranjeiras; Vila Célia; Vila Bandeirantes; Parque Peruche; Vila Vanda: Jardim São Bento; Jardim Ibéria; Jardim São Domingos; Jardim São Miguel; Vila Minozi; Imirim; Parque Léo; Vila Gouveia; Vila Rosin; Sítio do Mandaqui</t>
+  </si>
+  <si>
+    <t>Americanópolis
+Cidade Ademar
+Cidade Júlia
+Cupecê
+Jardim Cidália
+Jardim Cupecê
+Jardim Harmonia
+Jardim Los Angeles
+Jardim Luso
+Jardim Maria Luiza
+Jardim Martini
+Jardim Melo
+Jardim Miriam
+Jardim Niteroi
+Jardim Nosso Lar
+Jardim Orly
+Jardim Prudência
+Jardim Santo Antoninho
+Jardim São Carlos
+Jardim São Jorge
+Jardim Sônia
+Jardim Uberaba
+Jardim Vilas Boas
+Jardim Zaira
+Vila Capela
+Vila Castelo
+Vila Clara
+Vila Erna
+Vila Império
+Vila Inglesa
+Vila Joaniza
+Vila Marari
+Vila Nova Caledônia
+Vila Patrimonial
+Vila Rica
+Vila São Paulo</t>
+  </si>
+  <si>
+    <t>29.3</t>
+  </si>
+  <si>
+    <t>Chácara Meyer
+Chácara Monte Sol
+Cidade Dutra
+Conjunto Residencial Salvador Tolezani
+Granja Nossa Senhora Aparecida
+Jardim Alpino
+Jardim Amélia
+Jardim Ana Lúcia
+Jardim Angelina
+Jardim Beatriz
+Jardim Bichinhos
+Jardim Bonito
+Jardim Clipper
+Jardim Colonial
+Jardim Cristal
+Jardim Cruzeiro
+Jardim das Camélias
+Jardim das Imbuias
+Jardim das Praias
+Jardim do Alto
+Jardim Edilene
+Jardim Edith
+Jardim Floresta
+Jardim Graúna
+Jardim Guanabara
+Jardim Guanhembu
+Jardim Ícaraí
+Jardim Império
+Jardim Iporanga
+Jardim Jordanópolis
+Jardim Kika
+Jardim Kioto
+Jardim Lallo
+Jardim Leblon
+Jardim Mália
+Jardim Marcel
+Jardim Maria Rita
+Jardim Maringa
+Jardim Nizia
+Jardim Orion
+Jardim Panorama
+Jardim Pouso Alegre
+Jardim Presidente
+Jardim Primavera
+Jardim Progresso
+Jardim Quarto Centenário
+Jardim Real
+Jardim Rêgis
+Jardim Represa
+Jardim República
+Jardim Rio Bonito
+Jardim Rosalina
+Jardim Samambaia
+Jardim Santa Rita
+Jardim São Benedito
+Jardim São Rafael
+Jardim Satélite
+Jardim Toca
+Parque Alto
+Parque Atlântico
+Parque das Árvores
+Parque do Castelo
+Parque Esmeralda
+Parque Nações Unidas
+Parque Paulistinha
+Recanto dos Sonhos
+Rio Bonito
+Terceira Divisão de Interlagos
+Vila da Paz
+Vila Diana
+Vila Progresso
+Vila Quintana
+Vila Represa
+Vila Rubi
+Vila São José
+Vila Vera</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>Cidade Líder; Fazenda Aricanduva; Jardim Brasília; Jardim das Carmelitas; Jardim Eliane; Jardim Fernandes; Jardim Ipanema; Jardim Marília; Jardim Santa Maria; Jardim Santa Terezinha; Parque Savoy City; Vila Arisi; Vila Santa Rita.</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>Consolação, Higienópolis, Vila Buarque e Pacaembu</t>
+  </si>
+  <si>
+    <t>12.8</t>
+  </si>
+  <si>
+    <t>Água Funda
+Vila Água Funda
+Conjunto dos Bancários
+Bosque da Saúde (Parte Leste da Av. Dr. Ricardo Jafet)
+Vila Brasilina
+Vila Brasílio Machado
+Cursino
+Vila Firmiano Pinto
+Vila Gumercindo
+Vila Moraes
+Jardim Previdência
+Vila Santo Stefano
+Jardim São Miguel
+Parque da Saúde
+Saúde
+São Salvador
+Jardim da Saúde
+Vila Simões</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>Jardim Belém
+Jardim Keralux
+Jardim Matarazzo
+Jardim Verônia
+Parque Boturussu
+Parque Guedes
+Vila Císper
+Vila Guaraciaba (parte)
+Vila Nova Teresa
+Vila Paranaguá
+Vila Robertina
+Vila Sílvia (parte)</t>
+  </si>
+  <si>
+    <t>10.5</t>
+  </si>
+  <si>
+    <t>Chácara do Rosário;
+Chácara Domilice;
+Chácara Nossa Sra. Aparecida;
+Conj. Res. Prestes Maia;
+Itaberaba;
+Jardim Adélia;
+Jardim Cachoeira;
+Jardim Iracema;
+Jardim Maristela;
+Jardim Monjolo;
+Jardim Monte Alegre;
+Jardim Noêmia;
+Jardim São Marcos;
+Moinho Velho;
+Nossa Senhora do Ó;
+Pq. Dom Luís;
+Pq. Mandi;
+Pq. Monteiro Soares;
+Vila Acre;
+Vila Albertina;
+Vila Amélia;
+Vila Arcádia;
+Vila Bancária Munhoz;
+Vila Bela;
+Vila Bracáia;
+Vila Brito;
+Vila Bruna;
+Vila Cardoso;
+Vila Cavatton;
+Vila Cruz das Almas;
+Vila do Congo;
+Vila Dona América;
+Vila Gonçalves;
+Vila Hebe;
+Vila Iara;
+Vila Iório;
+Vila Ismênia;
+Vila Júlio César;
+Vila Manuel Lopes;
+Vila Mariliza;
+Vila Marilu;
+Vila Marina;
+Vila Miriam;
+Vila Morro Grande;
+Vila Morro Verde;
+Vila Nívea;
+Vila Palmeiras;
+Vila Peruccio;
+Vila Picinin;
+Vila Portuguesa;
+Vila Primavera;
+Vila Progresso;
+Vila Ramos;
+Vila Regina;
+Vila Sá e Silva;
+Vila Santa Delfina;
+Vila São Francisco;
+Vila São Vicente;
+Vila Schmidt;
+Vila Simões;
+Vila Siqueira;
+Vila Timóteo;
+Vila União;
+Vila Zulmira Maria.</t>
+  </si>
+  <si>
+    <t>Cantinho do Céu 
+Chácara Cocaia 
+BNH  
+Chácara do Sol 
+Chácara Lagoinha 
+Cidade Luz 
+Cipó do Meio
+Colônia do Grajaú
+Corujas
+Gaivotas 
+Grajaú 
+Ilha do Bororé
+Jardim Almeida Prado 
+Jardim Alvorada (Grajaú) 
+Jardim Arco-íris 
+Jardim Azano
+Jardim Belcito 
+Jardim Bonito 
+Jardim Borba Gato 
+Jardim Brasília 
+Jardim Campinas 
+Jardim Castro Alves 
+Jardim das Pedras (Grajaú)
+Jardim dos Manacás
+Jardim Edda
+Jardim Edi 
+Jardim Eliana 
+Jardim Ellus
+Jardim Gaivotas 
+Jardim Icaraí 
+Jardim Ideal 
+Jardim Itajaí 
+Jardim Itatiáia 
+Jardim Iporanga
+Jardim Jaú
+Jardim Labitary 
+Jardim Lucélia 
+Jardim Marilda
+Jardim Marisa 
+Jardim Mirna 
+Jardim Monte Alegre 
+Jardim Monte Verde
+Jardim Myrna 
+Jardim Noronha 
+Jardim Nossa Senhora Aparecida 
+Jardim Nova Tereza 
+Jardim Novo Horizonte 
+Jardim Novo Jaú 
+Jardim Novo Lar 
+Jardim Orbam 
+Jardim Planalto
+Jardim Porto Velho
+Jardim Prainha
+Jardim Progresso
+Jardim Recanto do Sol
+Jardim Reimberg 
+Jardim Sabiá (Grajaú) 
+Jardim Salinas 
+Jardim Samara (Grajaú) 
+Jardim Samas 
+Jardim Santa Bárbara
+Jardim Santa Fé 
+Jardim Santa Francisca
+Jardim Santa Francisca Cabrini 
+Jardim Santa Tereza 
+Jardim São Bernardo 
+Jardim São Pedro 
+Jardim São Remo 
+Jardim Sete de Setembro
+Jardim Shangri-lá 
+Jardim Sipramar 
+Jardim Tanay 
+Jardim Três Corações 
+Jardim Toca
+Jardim Varginha 
+Jardim Orion 
+Jardim Zilda
+Jordanopolis
+Lago Azul 
+Parada 57 
+Parque Alto
+Parque América 
+Parque Brasil 
+Parque Cocaia 
+Parque Deizy
+Parque Grajaú 
+Parque Manacá 
+Parque Novo Grajaú 
+Parque Planalto 
+Parque Residencial Cocaia
+Parelheiros
+Parque Santa Cecília
+Parque São José
+Parque São Miguel 
+Parque São Paulo 
+Parque Shangrilá 
+Recanto Marisa 
+Sítio Cocaia 
+Toca do Tatu 
+Vila Morais Prado 
+Vila Narciso
+Vila Nascente 
+Vila Natal
+Vila Rubi</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t>19.6</t>
+  </si>
+  <si>
+    <t>9.9</t>
+  </si>
+  <si>
+    <t>Vila Olímpia, Itaim Bibi, Brooklin Novo</t>
+  </si>
+  <si>
+    <t>Conjunto Habitacional A.E. Carvalho
+Conjunto Habitacional Águia de Haia
+Itaquera
+Jardim Adelaide
+Jardim Aurora
+Jardim Cleide
+Jardim Irene
+Jardim Itapemirim
+Jardim Liderança
+Jardim Naufal
+Jardim Norma
+Jardim Redil
+Jardim São João
+Limoeiro
+Parada XV de Novembro
+Parque Guarani
+Parque Sevilha
+Vila Bozzini
+Vila Brasil
+Vila Campanela
+Vila Carmosina
+Vila Caxambu
+Vila Corberi
+Vila Jussara
+Vila Klaunig
+Vila Regina
+Vila Santana
+Vila Suíça
+Vila Taquari
+Vila Verde</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>Americanópolis
+Jardim Anchieta
+Vila Babilônia
+Jardim Bom Clima
+Vila Campestre
+Vila Canaã
+Vila Capela
+Vila Celeste
+Vila Clara
+Jardim Costa Pereira
+Jardim Cunha Bueno
+Cidade Domitila
+Vila do Encontro
+Vila Facchini
+Vila Guarani
+Jardim Itacolomi
+Jardim Jabaquara
+Jabaquara
+Vila Parque Jabaquara
+Cidade Leonor
+Jardim Lourdes
+Vila Mascote
+Jardim Mendes Gaia
+Jardim Metropolitano
+Vila Mira
+Jardim Oriental
+Vila Paulista
+Vila Santa Catarina
+Jardim São Martinho
+Jardim Scaff
+Jardim Sul São Paulo
+Cidade Vargas
+Vila da Várzea</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>Vila Milagrosa; Vila Germinal; Jaçanã; Vila Constança; Jardim Modelo; Jardim Aliança; Vila Carolina; Vila Ester; Vila Laura; Vila Isabel; Jardim Cabuçu; Parque Edu Chaves; Jardim Guapira; Vila Nilo; Chácara São João; Vila Nova Galvão</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>Jardim Marisa, Jardim Piauí, Jardim Vieira, Vila Jaguara, Vila Nilva, Vila Piauí, Chácara São João; Jardim Cimobil; Vila Varanda; Vila Eleonora; Vila Santa Edwiges; Vila Aparecida Ivone; Jardim Ramos Freitas; Jardim Belaura; Vila Nova Jaguara; Parque Anhanguera</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Centro Industrial do Jaguaré, Super Quadra Jaguaré, Vila Nova Jaguaré, Parque Continental, Vila Graziela, Vila Jaguaré e Vila Lageado.</t>
+  </si>
+  <si>
+    <t>27.6</t>
+  </si>
+  <si>
+    <t>Jaraguá (Centro)
+Cidade D’Abril
+City Jaraguá
+Jardim Bandeirantes
+Jardim Ipanema
+Jardim Líder
+Jardim Pirituba
+Jardim Rincão
+Jardim São João
+Jardim Shangri-lá
+Jardim Vivan
+Parada de Taipas
+Parque Nações Unidas
+Parque Pan-Americano
+Parque Taipas
+Vila Chica Luísa
+Vila Hilda
+Jardim Zoológico
+Vila Nossa Senhora da Conceição
+Vila Aurora
+Vila Nova Parada</t>
+  </si>
+  <si>
+    <t>Alto da Baronesa
+Alto da Riviera
+Balneário Dom Carlos
+Baronesa
+Chácara Bandeirantes
+Chácara Flórida
+Chácara Santa Maria
+Chácara Sonho Azul
+Cidade Ipava
+Cumbica
+Estância Mirim
+Vila Remo
+Estância Tangará
+Jardim Ângela
+Jardim Aracati
+Jardim Boa Esperança
+Jardim Caiçara
+Jardim Capela
+Jardim Clara Regina
+Jardim Coimbra
+Vila Gilda
+Jardim Copacabana
+Jardim das Flores
+Jardim Europa
+Jardim Fraternidade
+Jardim Fujihara
+Jardim Guarujá
+Jardim Gustavo
+Jardim Herculano
+Jardim Horizonte Azul
+Jardim Imbé
+Jardim Kagohara
+Jardim Maria Emília
+Jardim Mariane
+Jardim Nakamura
+Jardim Planalto
+Jardim Ranieri
+Jardim Recreio
+Jardim Remo
+Jardim dos Reis
+Jardim Rio Douro
+Jardim Rosa Maria
+Jardim Santa Margarida
+Jardim Santa Zélia
+Jardim São João
+Jardim São José
+Jardim São Lourenço
+Jardim São Manuel
+Jardim Solange
+Jardim Sônia Regina
+Jardim Tamoio
+Jardim Tupi
+Jardim Turquesa
+Jardim União
+Jardim Vale Verde
+Jardim Vera Cruz
+Jardim Wanda
+Loteamento Vila do Sol
+M’Boi Mirim
+Miaimi Paulista
+Morro do Índio
+Parque Bologne
+Parque Boulogne
+Parque Cristina
+Parque das Cerejeiras
+Parque do Lago
+Parque Lago
+Parque Maria Alice
+Parque Novo Santo Amaro
+Parque Santa Barbara
+Parque Santo Amaro
+Parque Santo Antônio
+Parque Santo Edwiges
+Parque Universitário Espírita
+Sapato Branco
+Vila Bom Jardim
+Jardim Caiçara
+Vila Calu
+Vila Damasceno
+Vila Dom José
+Vila Dona Meta
+Vila Gilda
+Vila Jaci
+Vila Nagibe
+Vila Remo
+Vila Santa Lúcia
+Vila São Judas
+Vila do Sol</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>Jardim Paulista, Jardim América</t>
+  </si>
+  <si>
+    <t>Colônia
+Conjunto Habitacional Fazenda do Carmo
+Conjunto Residencial José Bonifácio
+Jardim Cibele
+Jardim Helena
+Jardim Ivete
+Jardim Jordão
+Jardim Morganti
+Jardim Pedra Branca
+Jardim São Pedro
+José Bonifácio
+Vila Gil
+Vila Santa Terezinha</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>Conjunto da Paz, Jardim Augusta, Jardim Aurora, Jardim Brigida, Jardim Campos, Jardim do Campo, Jardim Dona Deolinda, Jardim Etelvina, Jardim Fanganiello, Jardim Gianetti, Jardim Guaianases, Jardim Moreno, Jardim Nova Guaianases, Jardim São Paulo, Jardim Ubirajara, Lajeado, Núcleo Lajeado, Parque Guaianases, Vila Andes, Vila Chabilândia, Vila Fukuya, Conjunto Habitacional Juscelino Kubitschek, Vila Iolanda 1, Vila Lourdes, Vila Minerva e Vila Nancy</t>
+  </si>
+  <si>
+    <t>Alto da Lapa, Bela Aliança, Lapa, Lapa de Baixo, Parque Residencial da Lapa, Siciliano, Vila Anastácio, Vila Argentina, Vila Augusto, Vila Bela Aliança, Vila Carlina, Vila Ipojuca e Vila Romana</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>Bairro do Limão; Jardim Pereira Leite; Jardim das Graças; Vila Barbosa; Vila Siqueira; Vila Carolina; Vila Cristo Rei; Vila Diva; Vila Prado; Vila Santista; Jardim São Luís; Vila Caroline; Vila Santa Maria; Sítio do Morro; Jardim Tabor; Vila Morro Alto; Jardim Primavera; Casa Verde Alta; Chácara Morro Alto; Vila Marisbela; Jardim Marina; Vila Espanhola</t>
+  </si>
+  <si>
+    <t>13.2</t>
+  </si>
+  <si>
+    <t>Vila Santo Antônio; Jardim Pícolo; Conjunto Residencial Santa Terezinha; Parque Mandaqui; Chácara do Encosto; Vila Vitória Mazzei; Vila Aurora; Jardim Paraíso; Jardim Vieira de Carvalho; Jardim Ormendina; Jardim Sônia; Jardim Santa Inês; Conjunto Residencial Santo Antônio; Jardim Carlu; Vila Amélia; Vila Romero; Jardim Malba; Jardim Maninos; Vila Basiléa; Lauzane Paulista; Jardim Emília; Vila Santos; Jardim Flamingo; Parque Cantareira; Pedra Branca; Jardim Itatinga;</t>
+  </si>
+  <si>
+    <t>Banhado
+Bela Vista
+Capivari
+Cipó do Meio
+Chácara Sanni
+Emburá
+Parque Florestal Paulista
+Chácara Galo Azul
+Parque Internacional
+Chácara Itajaá
+Mambu
+Engenheiro Marsilac
+Evangelista de Sousa
+Gramado
+Jardim dos Eucaliptos
+Paiol
+Ponte Alta</t>
+  </si>
+  <si>
+    <t>Moema, Indianópolis, Jardim Lusitânia,  Vila Nova Conceição</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vila Hipódromo, Mooca, Alto da Mooca e Parque da Mooca.</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>Cidade Jardim
+Fazenda Morumbi
+Jardim d'Oeste
+Jardim Everest
+Jardim Guedala
+Jardim Leonor (parte)
+Jardim Morumbi
+Jardim Panorama
+Jardim Silvia
+Jardim Viana
+Jardim Vitória Régia
+Morumbi
+Paineiras
+Real Parque
+Vila Morumbi
+Vila Progredior
+Vila Tramontano</t>
+  </si>
+  <si>
+    <t>Barragem
+Bosque do Sol
+Casa Grande
+Chácara Ana
+Chácara Lago Grande
+Chácara Santo Hubertos
+Chácara São Sebastião
+Chácara São Silvestre
+Chácara Schunck
+Cidade Luz
+Cidade Nova América
+Cidade Satélite
+Colônia
+Condomínio Palmeiras
+Curucutu
+Embura
+Itaim de Parelheiros
+Jaceguava
+Jardim Aladim
+Jardim dos Álamos
+Jardim Almeida
+Jardim Alviverde
+Jardim Campo Belo
+Jardim das Fontes
+Jardim das Laranjeiras
+Jardim do Bosque
+Jardim do Centro
+Jardim Herplin
+Jardim Iporã
+Jardim Itaim
+Jardim Juçara
+Jardim Maria Amália
+Jardim Maria Borba
+Jardim Novo Parelheiros
+Jardim Paulo Afonso
+Jardim Progresso
+Jardim Ramala
+Jardim Santa Cruz
+Jardim Santa Teresinha
+Jardim Santa Fé
+Jardim São Joaquim
+Jardim São Norberto
+Jardim Papai Noel
+Jardim São Nicolau
+Jardim Silveira
+Jardim Vera Cruz
+Parque Terceiro Lago
+Parque Sumaré
+Parque Florestal
+Parque Recreio
+Praia Paulistana
+Rancho Alegre
+Recanto Campo Belo
+Recanto do Papai
+Sítio Casa Grande
+Sítio Santa Cecília
+Sítio Vale Verde
+Sumaré
+Vargem Grande
+Vila Bororé
+Vila Esperança
+Vila Isabel
+Vila Marcelo
+Vila Nova Esperança
+Vila Roschel</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>15.4</t>
+  </si>
+  <si>
+    <t>Jardim Santa Marcelina; Jardim Nossa Senhora do Carmo; Vila Carmosina (parte); Jardim Marabá; Fazenda Nossa Senhora Do Carmo; Vila Ana Cláudia; Vila São Vicente; Chácara Santa Amélia; Jardim Elian; Conjunto Habitacional Gleba do Pêssego.</t>
+  </si>
+  <si>
+    <t>18.7</t>
+  </si>
+  <si>
+    <t>Balneário Mar Paulista
+Balneário São Francisco
+Conjunto Residencial Ingai
+Eldorado (Mata Virgem)
+Guacuri
+Itatinga
+Jardim Aparecida
+Jardim Apurá
+Jardim Clélia
+Jardim Domitila
+Jardim Guacuri
+Jardim Itapura
+Jardim Nastari
+Jardim Pedreira
+Jardim Rubilene
+Jardim Santa Teresinha
+Jardim Selma
+Paque Dorotéia
+Parque Bandeirantes
+Parque Primavera
+Pedreira
+Praia Leblon
+Sete Praias
+Vila Babi
+Vila dos Andradas
+Vila Guacuri
+Vila Missionária
+Zavuvus</t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>Chácara da Penha, Conjunto Habitacional Chaparral, Engenheiro Trindade, Guaiaúna, Jardim América da Penha, Jardim Concórdia, Jardim Jáu (Parte), Jardim do Norte, Jardim Paula, Jardim Recreio, Parque Eduardo, Penha de França, Tiquatira, Vila Beatriz, Vila Carlos de Campos, Vila Centenário, Vila Esperança, Vila Eugênio, Vila Feliz, Vila Germaine, Vila Granada, Vila Laís, Vila Maluf, Vila Maria Amália, Vila Marieta, Vila Nova Granada, Vila Olívia, Vila Ré, Vila Salete, Vila Santana, Vila Santo Antônio, Vila São Geraldo e Vila Vera</t>
+  </si>
+  <si>
+    <t>Perdizes, Vila Pompéia, Vila Anglo Brasileira, Sumaré e Pacaembu</t>
+  </si>
+  <si>
+    <t>23.9</t>
+  </si>
+  <si>
+    <t>Chácara Maria Trindade
+Conjunto Habitacional Recanto dos Humildes
+Jardim Adelfiore
+Jardim do Russo
+Jardim dos Manacás
+Jardim Perus
+Loteamento Vitória Régia
+Perus
+Recanto Paraíso
+Sítio Areião
+Sítio Botuquara
+Vila Caiuba
+Vila Fanton
+Vila Hungaresa
+Vila Inácio
+Vila Malvina
+Vila Nova Perus
+Vila Perus
+Vila Rancho Alegre
+Vila Santa Cruz</t>
+  </si>
+  <si>
+    <t>Jardim das Bandeiras
+Jardim Europa
+Vila Madalena
+Vila Nogueira
+Jardim Paulistano
+Pinheiros
+Jardim das Rosas
+Sumarezinho</t>
+  </si>
+  <si>
+    <t>Piqueri e Jardim Íris
+Chácara Inglesa, Jardim Felicidade e Jardim São Ricardo
+Vila Pereira Barreto e Vila Bonilha
+Vila Comercial, Jardim Líbano e City Pinheirinho
+Jardim Cidade Pirituba, Vila Zatt e Vila Mirante
+Jardim Paquetá, Vila Renato e Canta Galo
+Vila Pirituba, Jardim Santa Mônica e Vista Verde
+Jardim Regina, City Recanto Anastácio e Vila Clarice
+Vila Jaraguá e Jardim Monte Alegre</t>
+  </si>
+  <si>
+    <t>17.1</t>
+  </si>
+  <si>
+    <t>Burgo Paulista
+Jardim Cotinha
+Jardim Lisboa
+Jardim Laone
+Jardim Ponte Rasa
+Jardim Popular
+Jardim Soraia
+Jardim Três Marias
+Vila Constança
+Vila Costa Melo
+Vila Domitila
+Vila Fidelis Ribeiro
+Vila Frugoli
+Vila Ponte Rasa
+Vila Rio Branco
+Vila Sampaio
+Vila São Francisco
+Vila União</t>
+  </si>
+  <si>
+    <t>Cohab Educandário
+• Cohab Raposo Tavares
+• Conjunto Promorar Raposo Tavares
+• Educandário
+• Jardim Amaralina
+• Jardim Arpoador
+• Jardim Batalha
+• Jardim Boa Vista
+• Jardim Cambará
+• Jardim Cláudia
+• Jardim das Esmeraldas
+• Jardim Dracena
+• Jardim Educandário
+• Jardim Gilda Maria
+• Jardim Guaraú
+• Jardim João XXIII
+• Jardim Lago
+• Jardim Lúcia
+• Jardim Lúcio de Castro
+• Jardim Luiza
+• Jardim Maria Augusta
+• Jardim Monte Belo
+• Jardim Paulo VI
+• Jardim Raposo Tavares
+• Jardim Rosa Maria
+• Jardim Rubini
+• Jardim Rúbio
+• Jardim São Jorge
+• Jardim Uirapuru
+• Parque Ipê
+• Raposo Tavares
+• Vila Borges
+• Vila Maria Augusta</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>Anhangabaú
+República
+Santa Ifigênia</t>
+  </si>
+  <si>
+    <t>9.7</t>
+  </si>
+  <si>
+    <t>Jardim Ana Maria
+Jardim Botucatu
+Jardim Celeste
+Jardim Clímax
+Jardim dos Bandeirantes
+Jardim Elísio
+Cidade Nova Heliópolis
+Jardim Imperador
+Jardim Leônidas Moreira
+Jardim Liar
+Jardim Maria Estela
+Jardim Natália
+Jardim Patente
+Jardim Patente Novo
+Jardim Santa Cruz
+Jardim Santa Emília
+Jardim Santo Antônio do Cursino
+Jardim Seckler
+Jardim Tropical
+Parque Bristol
+Jardim São Savério
+São João Clímaco
+Vila Anchieta
+Vila Arapuã
+Vila Bandeirantes
+Vila Caraguatá
+Vila Conde do Pinhal
+Vila Cristália
+Vila Cristina
+Vila das Mercês
+Vila Elísio
+Vila Henrique Cunha Bueno
+Vila Liviero
+Vila Marte
+Vila Moinho Velho
+Vila Moraes
+Vila Natália
+Vila Quaquá
+Sacomã
+Vila Romano
+Vila Sacomã
+Vila Santa Teresa
+Vila Vera
+Vila Vergueiro
+Vila Vermelha</t>
+  </si>
+  <si>
+    <t>Campos Elíseos
+Santa Cecília</t>
+  </si>
+  <si>
+    <t>15.7</t>
+  </si>
+  <si>
+    <t>Jardim Abrantes
+Jardim Alice
+Vila Almeida
+Alto da Boa Vista
+Jardim Bela Vista
+Vila Campos Sales
+Vila Caravelas
+Jardim Cedro do Líbano
+Jardim Cordeiro
+Vila do Cruzeiro
+Jardim Dom Bosco
+Vila Elvira
+Jardim Dos Estados
+Chácara Flora
+Jardim Florida
+Conjunto Residencial Glória
+Granja Julieta
+Vila Guaianases
+Jardim Heliomar
+Vila Henrique
+Jardim Hípico
+Vila Internacional
+Vila Ipé
+Chácara Japonesa
+Vila Kostka
+Jardim Martini
+Vila Miranda
+Chácara Monte Alegre
+Chácara Paineiras
+Jardim Petrópolis
+Chácara Pouso Alegre
+Jardim Promissão
+Santo Amaro
+Jardim Santo Amaro
+Chácara Santo Antônio
+Jardim Santo Antonio
+Vila São Francisco
+Chácara São Luiz
+Vila União Várzea de Baixo
+Jardim Várzea de Baixo</t>
+  </si>
+  <si>
+    <t>City América
+Parque São Domingos
+Vila Boaçava
+Vila Fiat Lux
+Parque Maria Domitila
+Vila Mangalot
+Jardim Mangalot
+Jardim Santo Elias
+Vila Jaguari
+Jardim Nardini
+Vila Jaraguá
+Jardim Jaraguá
+Parque Anhanguera
+Vila Nova Esperança
+Vila Guedes
+Vila Soares
+Jardim Vista Linda
+Jardim Mutinga
+Jardim Maristela
+Vila Maria Eugênia
+Vila Zulmira</t>
+  </si>
+  <si>
+    <t>ardim Silveira (parte); Vila Charlote; Vila Rosa; Vila Raquel; Vila Ivone; Vila Margarida; Jardim Sofia; Vila Florinda; Vila Ema; Vila Santo Antônio; Vila Angelina; Vila Norma; Jardim Theália; Vila Amadeu; Vila São Domingos; Vila Carmem; Parque Tomás Saraiva; Jardim Independência; Jardim Tereza; Vila Darli; Jardim Central; Jardim Otília; Vila Mercedes; Vila Mirtes; Jardim São Lourenço; Jardim Dias; Vila Paulo Silas; Vila Santa Virgínia; Vila Moça; Vila Central; Vila Divina Pastora; Parque São Lucas; Sítio Pinheirinho; Vila Anadir; Cidade Continental; Jardim Guairacá; Vila Heloísa; Jardim Redenção; Vila Cleonice; Vila Moderna; Vila Arlinda; Vila Nova Pauliceia; Parque Residencial Oratório; Vila Merly; Vila Nair; Vila Ivg; Vila Lavínia; Vila Ana Clara; Vila Else; Vila Miami; Vila Rosicler; Jardim Panorama; Vila Industrial; Vila São Nicolau; Vila Mendes; Vila Cunha Bueno; Vila Iguaçu; Vila Nova Utinga; Parque Pereira</t>
+  </si>
+  <si>
+    <t>Cidade Centenário
+Cidade São Mateus
+Cidade Satélite Santa Bárbara
+Jardim Cinco de Julho
+Jardim Egle
+Jardim Imperador
+Jardim Itápolis
+Jardim Nove de Julho
+Jardim Paraguaçu
+Jardim Ricardo
+Jardim Santa Adélia
+Jardim São Cristóvão
+Jardim São José
+Jardim Tietê
+Jardim Três Marias
+Jardim Valquiria
+Parque Colonial
+Parque Industrial São Lourenço
+São Mateus</t>
+  </si>
+  <si>
+    <t>Jardim Nair; Jardim Lapena; São Miguel Paulista (bairro); Vila Nova Itaquera de Baixo; Cidade Nitro Operária; Vila Siqueira; Vila Pedroso; Vila Americana; Vila Doutor Eiras; Parque Sônia; Vila São Silvestre; Vila Jacuí, Vila Giordano; Cidade São Miguel; Vila Sinhá; Vila Rosária; Vila Vessoni; Vila Aparecida; Vila Olho D’Água; Cidade Nova São Miguel; Jardim São Sebastião; Vila Xavantes; União de Vila Nova; Jardim Ipanema; Jardim Lucinda; Vila Raquel; Vila Progresso; Jardim Beatriz; Vila Danúbio Azul; Jardim Ubirajara.</t>
+  </si>
+  <si>
+    <t>Carrãozinho
+Conjunto Promorar Rio Claro
+Jardim Alto Alegre
+Jardim Bandeirante
+Jardim Buriti
+Jardim Colorado
+Jardim Rodolfo Pirani
+Jardim Santo André
+Jardim São Francisco
+Jardim São João
+Jardim Vera Cruz
+Jardim Vila Carrão
+Núcleo Residencial Morro do Sabão
+Parque das Flores
+Parque São Rafael
+Vila Bela
+Vila Ester</t>
+  </si>
+  <si>
+    <t>13.4</t>
+  </si>
+  <si>
+    <t>Barreira Grande; Jardim Colorado; Jardim Barreira Grande; Jardim Porteira Grande; Vila Bancária; Vila Primavera; Conj. Hab. Vila Prudente; Vila Júlio; Vila Orlando; Vila União; Vila Nova; Vila Ester; Jardim Ana Rosa; Vila Brasil; Jardim Luzitano; Vila Sirene; Vila Virgínia; Vila Tolstói; Sapopemba; Vila Fátima; Jardim Soares; Vila Luso Brasileira; Jardim Clara Regina; Parque São Lourenço; Vila Guiomar; Jardim Amaro; Jardim Ângela; Jardim Mimar; Jardim Ivone; Jardim Iguaçu; Jardim Alzira; Cohab Vila Flórida; Jardim Iva; Parque Bancário; Jardim Grimaldi; Jardim Dona Sinhá; Jardim Paraguaçu; Conj. Res. Jardim Centenário; Parque Luís Mucciolo; Vila Portuguesa; Parque Lar Nacional; Conj. Hab. Teotônio Vilela; Jardim Sapopemba; Jardim Planalto; Parque Santa Madalena; Jardim Elba; Parque do Jardim Sapopemba (parte); Jardim Walquiria; Vila Renato; Jardim Adutora; Vila Cardoso Franco; Conj. Res. Sítio do Oratório; Jardim São Roberto; Conj. Hab. Mascarenhas de Morais; Fazenda da Juta; Conj. Hab. Itaquera B2; Conj. Hab. Itaquera B3; Conj. Hab. do Juta.</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Anhangabaú
+Parque Dom Pedro I
+Mercado
+Sé</t>
+  </si>
+  <si>
+    <t>Interlagos
+Jardim Bessa
+Vila Califórnia
+Capela do Socorro
+Jardim Cristina
+Vila Franca
+Vila Friburgo
+Jardim Guarapiranga
+Parque Interlagos
+Jardim Ipanema
+Jardim do Lago
+Vila Lisboa
+Jardim Mara
+Jardim Marabá
+Jardim Nova Guarapiranga
+Jardim Paquetá
+Parque Rony
+Jardim Santa Helena
+Jardim São Jorge
+Jardim São José de Guarapiranga
+Socorro
+Jardim Socorro
+Vila Socorro
+Jardim Suzana
+Jardim Tereza
+Jardim Três Marias
+Veleiros
+Jardim Veneza</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>56.3</t>
+  </si>
+  <si>
+    <t>Tremembé, Vila Nova Mazzei; Jardim Floresta; Parque Palmas do Tremembé; Jardim Hugo; Jardim Yara; Jardim Maria Nazaré; Jardim Entre Serras; Jardim Virgínia Bianca; Jardim da Ponte; Parque Ramos de Freitas; Vila Santa Maria; Vila Vieira; Parque do Tremembé; Vila Esmeralda; Jardim Santa Marcelina; Jardim Daysy; Jardim Ibira; Jardim Ibiratiba; Vila Marieta; Vila Bibi; Vila Albertina; Jardim Denise; Vila Maria Augusta; Vila Irmãos Arnoni; Vila dos Rosas; Jardim São Manoel; Parque Petrópolis; Vila Solear: Vila Pereira; Vila Brasil; Jardim Guapira (parte); Jardim das Rosas; Vila Paulistana; Jardim Filhos da Terra; Bortolândia; Parque Casa de Pedra; Jardim Apuanã; Jardim Jaçanã; Jardim Mário Fonseca; Jardim Joamar; Vila Aurora; Vila Zilda; Conj. Fidalgo; Jardim Tremembé; Jardim M Maurício; Jardim Maria Cândida; Jardim Ataliba Leonel; Vila Fidalgo; Vila Dornas; Jardim Luísa; Vila Virgínia; Jardim Piqueri; Jardim Furnas; Jardim Francisco Mentem; Jardim Joana D’Arc; Jardim Martins Silva; Jardim Campo Limpo; Jardim Fontalis; Vila Ayrosa; Jardim Flor de Maio; Chácara São José; Jardim Corisco; Jardim das Pedras; Sítio São João; Chácara Paraíso; Chácara Santa Sofia; Chácara São Francisco; Jardim Recanto Verde; Jardim Uniserve; Jardim Valparaíso; Jardim Labitary;</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>Vila Dom Pedro II, Parada Inglesa, Jardim França, Vila Mazzei, Jardim Kerlakian, Jardim Barro Branco, Jardim Dona Leonor Mendes de Barros, Jardim Maria Antônia, Parque Rodrigues Alves, Tucuruvi, Vila Pedrosa, Vila Gustavo, Vila Nivi, Vila Constança, Vila Santa Terezinha, Parque Vitória e Vila Cachoeira</t>
+  </si>
+  <si>
+    <t>10.3</t>
+  </si>
+  <si>
+    <t>Jardim Ampliação
+Jardim Fonte do Morumbi
+Jardim Parque Morumbi
+Jardim Santo Antônio
+Jardim Vitória Régia
+Panamby
+Paraíso do Morumbi
+Paraisópolis
+Parque Bairro do Morumbi
+Parque do Morumbi
+Retiro Morumbi
+Vila Andrade
+Vila das Belezas
+Vila Ernesto
+Vila Palmas
+Vila Plana
+Vila Susana</t>
+  </si>
+  <si>
+    <t>Chácara Figueira Grande
+Jardim Bartira
+Jardim Campos
+Jardim Carolina
+Jardim dos Ipês
+Jardim Eva
+Jardim Heloisa
+Jardim Miragaia
+Jardim Nazareth
+Jardim Quisisana
+Jardim Robrú
+Jardim Rosina
+Jardim Santo Antônio
+Jardim Santo Elias
+Jardim Senice
+Vila Clara
+Vila Conceição
+Vila Curuçá Velha
+Vila Luzimar
+Vila Nova Curuçá
+Vila Raquel
+Vila Simone
+Vila Stela</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>Capão do Embira
+Chácara Belenzinho
+Jardim Anália Franco
+Jardim Iara
+Jardim Têxtil (parte)
+Parque Cruzeiro do Sul
+Vila Antonina
+Vila Araci
+Vila Cruzeiro
+Vila Formosa
+Vila Guarani
+Vila Mafra
+Vila Matias
+Vila Olinda</t>
+  </si>
+  <si>
+    <t>Vila Guilherme; Vila Isolina Mazzei; Vila Salvador Romeu; Vila Isolina; Vila Paiva; Vila Santa Catarina; Jardim da Coroa; Vila Pizzotti; Vila Eleonore; Vila Bariri; Vila Leonor; Chácara Cuoco; Parque Velloso; Jardim da Divisa;</t>
+  </si>
+  <si>
+    <t>Conjunto Araucária
+Jardim Alto Pedroso
+Jardim da Casa Pintada
+Jardim das Camélias
+Jardim Matarazzo
+Jardim Planalto
+Jardim Pedro José Nunes
+Jardim Ruth
+Jardim Santa Maria
+Jardim Santana
+Jardim São Carlos
+Limoeiro
+Parque Cruzeiro do Sul
+Vila Amália
+Vila Carolina
+Vila Jacuí
+Vila Monte Santo
+Vila Norma
+Vila Reis
+Vila Santa Inês
+Vila Síria
+União de Vila Nova</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>Conjunto Haddad
+Jardim Humaitá
+Jardim São Ricardo
+Parque da Lapa
+Vila Hamburguesa
+Vila Leopoldina
+Vila Ribeiro de Barros</t>
+  </si>
+  <si>
+    <t>11.8</t>
+  </si>
+  <si>
+    <t>Vila Maria; Jardim Japão; Vila Maria Alta; Vila Maria Baixa; Parque Vila Maria; Parque Novo Mundo; Jardim Andaraí; Conjunto Promorar Vila Maria</t>
+  </si>
+  <si>
+    <t>Vila Mariana
+Vila Clementino até a rua Loefgreen
+Chácara do Castelo
+Chácara Klabin / Jardim Vila Mariana
+Conjunto dos Bancários
+Jardim Aurélia
+Jardim da Glória
+Jardim Lutfalla
+Paraíso até a Rua Tutoia
+Vila Afonso Celso</t>
+  </si>
+  <si>
+    <t>Vila Aricanduva; Chácara 6 de Outubro; Vila Euthália; Vila Dalila; Jardim Maringá; Vila Talarico; Vila Nova Savoia; Vila Guilhermina; Jardim Triana; Jardim Assunção; Jardim Samara; Jardim São João; Jardim Hercília; Vila Palmeirinha; Cidade Patriarca</t>
+  </si>
+  <si>
+    <t>Vila Medeiros, Vila Sabrina, Vila Ede, Vila Munhoz, Jardim Brasil, Jardim Guançã, Jardim Julieta, Conjunto Promorar Fernão Dias, Jardim Neida, Vila Alegria, Vila Elisa, Vila Luísa</t>
+  </si>
+  <si>
+    <t>Vila Prudente; Vila Alpina; Vila Zelina; Vila São Maurício; Vila Haddad; Vila Santa Teresa; Vila São Carlos; Quinta da Paineira; Parque Lituânia; Vila Alois; Conj. Hab. Cintra Gordinho; Parque da Vila Prudente; Vila Bela; Vila Lúcia; Jardim Avelino; Vila Macedópolis; Vila Califórnia</t>
+  </si>
+  <si>
+    <t>Conjunto Residencial do Morumbi
+Ferreira
+Jardim Alvorada
+Jardim Celeste (parte)
+Jardim Colombo
+Jardim das Vertentes
+Jardim Jaqueline
+Jardim Jussara
+Jardim Leila
+Jardim Leonor (parte)
+Jardim Londrina
+Jardim Monte Kemel
+Jardim Olympia
+Jardim Peri Peri (parte)
+Jardim Taboão
+Jardim Trussardi
+L'Habitare
+Lar São Paulo
+Superquadra Morumbi
+Vila Albano
+Vila Inah
+Vila Morse
+Vila Sônia
+Vila Susana</t>
+  </si>
+  <si>
+    <t>Bom Retiro
+Luz
+Ponte Pequena</t>
+  </si>
+  <si>
+    <t>Cambuci
+Vila Deodoro</t>
+  </si>
+  <si>
+    <t>Brás
+Mercado</t>
+  </si>
+  <si>
+    <t>Campininha
+Campo Grande
+Conjunto Residencial Sabará
+Jardim Alva
+Jardim Anhanguera
+Jardim Bélgica
+Jardim Campo Grande
+Jardim Consórcio
+Jardim da Campina
+Jardim Diomar
+Jardim do Carmo
+Jardim dos Prados
+Jardim Ernestina
+Jardim Jua
+Jardim Luanda
+Jardim Marajoara
+Jardim Palmares
+Jardim Sabará
+Jardim Santa Cruz
+Jardim Taquaral
+Jardim Ubirajara
+Jardim Umuarama
+Jurubatuba
+Parque Residencial Júlia
+Usina Piratininga
+Vila Agueda
+Vila Almeida
+Vila Anhanguera
+Vila Arriete
+Vila Baby
+Vila Campo Grande
+Vila do Castelo
+Vila Emir
+Vila Gea
+Vila Isa
+Vila Santana
+Vila São Pedro
+Vila Sofia</t>
+  </si>
+  <si>
+    <t>Chácara Pirajussara
+Horto do Ipê
+Jardim Ana Maria
+Jardim Bom Refúgio
+Jardim Campo Limpo
+Jardim Catanduva
+Jardim Elisa
+Jardim Elizabeth
+Jardim Faria Lima
+Jardim Helga
+Jardim Ingá
+Jardim Iracema
+Jardim Itamaraty
+Jardim Jamaica
+Jardim Laranjal
+Jardim Leme
+Jardim Leônidas Moreira
+Jardim Marcelo
+Jardim Maria Duarte
+Jardim Maria Sampaio
+Jardim Maria Virgínia
+Jardim Martinica
+Jardim Mitsutani
+Jardim Nadir
+Jardim Olinda
+Jardim Paris
+Jardim Piracuama
+Jardim Pirajussara
+Jardim Prestes Maia
+Jardim Rebouças
+Jardim Roni
+Jardim Rosana
+Jardim Samara
+Jardim Santa Efigênia
+Jardim São Januário
+Jardim São Mateus
+Jardim São Roque
+Jardim Umarizal
+Jardim Umuarama
+Parque Arariba
+Parque Esmeralda
+Parque Flamengo
+Parque Jardim Mirassol
+Parque Munhoz
+Parque Rebouças
+Parque Regina
+Pirajussara
+Residencial Morumbi
+Umarizal
+Vila Alteza
+Vila América
+Vila Anália
+Vila Brasil
+Vila Carioca
+Vila França
+Vila Nova Pirajussara
+Vila Pirajussara
+Vila Rica</t>
+  </si>
+  <si>
+    <t>Capão Redondo
+Capelinha
+Cidade Auxiliadora
+Cohab Monet
+Conjunto Habitacional Instituto Adventista
+Conjunto Habitacional JD São Bento
+Conjunto Habitacional Pirajussara
+Jardim Albano
+Jardim Alvorada
+Jardim Amália
+Jardim Atlântico
+Jardim Aurélio
+Jardim Avenida
+Jardim Boa Esperança
+Jardim Bom Pastor
+Jardim Campo de Fora
+Jardim Campo dos Ferreiros
+Jardim Capão Redondo
+Jardim Clarice
+Jardim Clélia
+Jardim Comercial
+Jardim das Rosas
+Jardim do Colégio
+Jardim Dom José
+Jardim Eledi
+Jardim Eledy
+Jardim Iae
+Jardim Ipê
+Jardim Irapiranga
+Jardim Irene
+Jardim Itaóca
+Jardim Janiópolis
+Jardim Jeriva
+Jardim Lídia
+Jardim Lilah
+Jardim Macedônia
+Jardim Madalena
+Jardim Maracá
+Jardim Modelo
+Jardim Mônica
+Jardim Nova Germânia
+Jardim Sagrado Coração
+Jardim Sandra
+Jardim São Bento Novo
+Jardim Sônia Inga
+Jardim Vale das Virtudes
+Jardim Valquiria
+Parque do Engenho
+Parque Fernanda
+Parque Independência
+Parque Ligia
+Parque Maria Helena
+Parque Residencial Bandeirante
+Parque Sônia
+Parque Vera Cruz
+Valo Velho
+Vila das Belezas
+Vila Fazzeoni
+Vila Fazzione
+Vila Maringá
+Vila Rosina
+Vila Santa Maria</t>
+  </si>
+  <si>
+    <t>Barra
+Barra Três Poderes
+Barro Branco
+Castro Alves
+Cidade Tiradentes
+Conjunto Habitacional Barro Branco I
+Conjunto Habitacional Barro Branco II
+Ferroviários
+Gráficos
+Inácio Monteiro
+Jardim dos Pereiras
+Jardim Monte Verde
+Jardim Pérola
+Jardim Pérola II
+Jardim Pérola III
+Jardim São Raimundo
+Jardim Souza Ramos
+Jardim Wilma Flor
+Nascer do Sol
+Passagem Funda
+Pérola Vitória
+Prestes Maia
+Profeta Geremias
+Santa Etelvina
+Santa Etelvina – Metalúrgicos
+Setor G
+Sitio Conceição
+Vila Paulista
+Vila Yolanda</t>
+  </si>
+  <si>
+    <t>Cidade Popular
+Conjunto Habitacional Juscelino Kubitschek
+Guaianases
+Jardim Aurea
+Jardim do Divino
+Jardim Marilena
+Jardim Marpu
+Jardim São Carlos
+Jardim São Domingos
+Jardim São João
+Jardim São Paulo
+Jardim São Paulo Novo
+Jardim São Paulo Velho
+Jardim Soares
+Parque Central
+Vila ABC
+Vila Aurea
+Vila Bela Vista
+Vila Buenos Aires
+Vila Cosmopolita
+Vila Marilena
+Vila Popular
+Vila Princesa Isabel
+Vila Roseira
+Vila Santa Cruz
+Vila São Geraldo
+Vila São José
+Vila Solange
+Vila Zefira</t>
+  </si>
+  <si>
+    <t>Iguatemi
+Jardim Alto Alegre
+Jardim Arantes
+Jardim Augusto
+Jardim Conquista
+Jardim da Laranjeira
+Jardim das Rosas
+Jardim Iguatemi
+Jardim Laranjeiras
+Jardim Limoeiro
+Jardim Maria Lídia
+Jardim Marilu
+Jardim Ricardo
+Jardim Roseli
+Jardim São Benedito
+Jardim São Gonçalo
+Núcleo Residencial São João
+Palanque
+Parque Boa Esperança
+Recanto Alegre
+Recanto Verde do Sol
+Terceira Divisão
+Vila Palma</t>
+  </si>
+  <si>
+    <t>Alto do Ipiranga
+Dom Pedro I
+Ipiranga
+Vila Carioca
+Vila Eulália
+Vila Firmiano Pinto
+Vila Independência
+Vila Monumento
+Vila São José</t>
+  </si>
+  <si>
+    <t>Chácara Dona Olívia
+Cidade Kemel
+Conjunto Encosta Norte
+Fazenda Itaim
+Itaim Paulista
+Jardim Aimoré
+Jardim Benfica
+Jardim Camargo Novo
+Jardim Camargo Velho
+Jardim Dalmo
+Jardim das Oliveiras
+Jardim Elza
+Jardim Eva
+Jardim Ida Guedes
+Jardim Indaiá
+Jardim Jaraguá
+Jardim Laura
+Jardim Mabel
+Jardim Meliunas
+Jardim Miragaia
+Jardim Miriam
+Jardim Nélia
+Jardim Progresso
+Jardim São Luís
+Jardim Sílvia
+Jardim Tuã
+Jardim Vilma
+Loteamento Santana do Agreste
+Parque Amélia
+Parque Santa Amélia
+Vila Alabama
+Vila Carolina
+Vila Escolar
+Vila Itaim
+Vila Jurema
+Vila Luzimar
+Vila Margareth
+Vila Melo
+Vila Morgadouro
+Vila Neila
+Vila São José
+Vila Sérgio
+Vila Silva Teles
+Vila Valdemar</t>
+  </si>
+  <si>
+    <t>Chácara Três Meninas
+Cidade Nitro Química
+Jardim Célia
+Jardim Dom Fernando
+Jardim Fluminense
+Jardim Ideal
+Jardim Maia
+Jardim Margarida
+Jardim Noemia
+Jardim Romano
+Jardim São Martinho
+Parque Paulistano
+Vila Aimoré
+Vila Itaim
+Vila Mara
+Vila Piracicaba
+Vila Seabra
+Vila Vitória</t>
+  </si>
+  <si>
+    <t>Chácara Figueira Grande
+Chácara Nossa Senhora do Bom Conselho
+Chácara Santana
+Chácara Três Caravelas
+Chácara Vista Alegre
+Cidade Fim de Semana
+Conjunto Promorar São Luís
+Copacabana
+Guarapiranga
+Itupu
+Jardim Alfredo
+Jardim Boa Vista
+Jardim Bronzato
+Jardim Capelinha
+Jardim Casablanca
+Jardim Cristália
+Jardim Dulce
+Jardim Duprat
+Jardim Fim de Semana
+Jardim Flores
+Jardim Flórida Paulista
+Jardim Francisco
+Jardim Germânia
+Jardim Ibirapuera
+Jardim Leni
+Jardim Leonardo
+Jardim Letícia
+Jardim Marco Paulo
+Jardim Marquesa
+Jardim Mazza
+Jardim Mirante
+Jardim Monte Azul
+Jardim Nagib Salem
+Jardim Nair
+Jardim Neide
+Jardim Novo Santo Amaro
+Jardim Riviera
+Jardim Santa Edwiges
+Jardim Santa Gertrudes
+Jardim Santa Josefina
+Jardim São Francisco de Assis
+Jardim São Joaquim
+Jardim São Luís
+Jardim Sousa
+Jardim Thomaz
+Jardim Tomas
+Jardim Vaz de Lima
+Jardim Vergueiro
+Jardim Ymay
+Parque Alves de Lima
+Parque do Otero
+Parque Europa
+Parque Paiolzinho
+Parque Santo Antonio
+Peninha
+Piraporinha
+Praia Azul
+Praia da Lagoa
+Recanto Santo Antônio
+Riviera Paulista
+São Luís
+Vila Belezas
+Vila Maracanã
+Vila Michelina
+Vila Prel</t>
+  </si>
+  <si>
+    <t>Aclimação
+Glicério
+Liberdade</t>
+  </si>
+  <si>
+    <t>Alto da Pari
+Canindé
+Pari</t>
+  </si>
+  <si>
+    <t>Cidade São Francisco
+Jardim Adalgisa
+Jardim Califórnia
+Jardim Centenário
+Jardim D’Abril
+Jardim Dinorah
+Jardim do Lago
+Jardim dos Cataldis
+Jardim Esmeralda
+Jardim Esther
+Jardim Esther Yolanda
+Jardim Farah
+Jardim Gilberto
+Jardim Imperial
+Jardim Ivana
+Jardim Julieta
+Jardim Maria Lúcia
+Jardim Maria Luiza
+Jardim Nelly
+Jardim Odete
+Jardim Rio Pequeno
+Jardim Santos Dumont
+Jardim Sarah
+Jardim Tropical
+Parque dos Príncipes
+Parque Malagoli
+Parque Rio Pequeno
+Rio Pequeno
+Vila Alba
+Vila Antônio
+Vila Butantã
+Vila Dalva
+Vila Dinorah
+Vila Esther
+Vila Invernada
+Vila Madeiral
+Vila Nova Alba
+Vila Polopoli
+Vila Popo Poli
+Vila Ramos
+Vila São Domingos
+Vila São Francisco
+Vila São Luís
+Vila São Silvestre
+Vila Sol
+Vila Tiradentes
+Vila Universitária
+Vila Vasconcelos</t>
+  </si>
+  <si>
+    <t>Chácara Inglesa
+Mirandópolis
+Parque Imperial
+Planalto Paulista
+São Judas
+Saúde
+Vila Cruzeiro do Sul
+Vila do Bosque
+Vila Monte Alegre</t>
+  </si>
+  <si>
+    <t>Água Fria
+Chora Menino
+Imirim
+Jardim Carmen Verônica
+Jardim do Colégio
+Jardim Guanandi
+Jardim São Paulo
+Parque Anhembi
+Santa Terezinha
+Santana
+Sítio Pedra Branca
+Vila Bianca
+Vila José Casa Grande
+Vila Mariza Mazzei
+Vila Matias
+Vila Paulicéia
+Vila Rabelo
+Vila Santa Luzia
+Vila Santana
+Vila Siciliano
+Vila Zélia</t>
+  </si>
+  <si>
+    <t>Chácara Maranhão
+Chácara Nani
+Cidade Mãe do Céu
+Jardim Alice
+Jardim Textília
+Maranhão
+Parque São Jorge
+Tatuapé
+Vila Azevedo
+Vila Brasil
+Vila Gomes Cardim
+Vila Luiza
+Vila Luzitana
+Vila Moreira
+Vila Santo Estevão</t>
   </si>
 </sst>
 </file>
@@ -365,8 +2362,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,794 +2705,1378 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567F9104-819A-6C4A-B2B3-7BA5B21804E4}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>3550308001</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>3550308002</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>3550308003</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>3550308004</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>3550308005</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>3550308006</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>3550308007</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>3550308008</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>3550308009</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>3550308010</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>3550308011</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="2">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>3550308012</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>3550308013</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>3550308014</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <v>3550308015</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>3550308016</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>3550308017</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>3550308018</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="2">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>3550308019</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>3550308020</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>3550308021</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>3550308022</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="2">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>3550308023</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>3550308024</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
         <v>3550308025</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="2">
+        <v>15</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
         <v>3550308026</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
         <v>3550308027</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
         <v>3550308028</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>3550308029</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>3550308030</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="2">
+        <v>92</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>3550308031</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
         <v>3550308032</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
         <v>3550308033</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>3550308034</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36">
         <v>3550308035</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="2">
+        <v>15</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37">
         <v>3550308036</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="2">
+        <v>14</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38">
         <v>3550308037</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39">
         <v>3550308038</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
         <v>3550308039</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
         <v>3550308040</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
         <v>3550308041</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43">
         <v>3550308042</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" s="2">
+        <v>37</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44">
         <v>3550308043</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45">
         <v>3550308044</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46">
         <v>3550308045</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" s="2">
+        <v>24</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47">
         <v>3550308046</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48">
         <v>3550308047</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49">
         <v>3550308048</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" s="2">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50">
         <v>3550308049</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51">
         <v>3550308050</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D51" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52">
         <v>3550308051</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53">
         <v>3550308052</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" s="2">
+        <v>200</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
         <v>3550308053</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" s="2">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55">
         <v>3550308054</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56">
         <v>3550308055</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57">
         <v>3550308056</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" s="2">
+        <v>153</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58">
         <v>3550308057</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59">
         <v>3550308058</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D59" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60">
         <v>3550308059</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61">
         <v>3550308060</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62">
         <v>3550308061</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63">
         <v>3550308062</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64">
         <v>3550308063</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" s="2">
+        <v>8</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65">
         <v>3550308064</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66">
         <v>3550308065</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66" s="2">
+        <v>7</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67">
         <v>3550308066</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68">
         <v>3550308067</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69">
         <v>3550308068</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70">
         <v>3550308069</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70" s="2">
+        <v>14</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71">
         <v>3550308070</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72">
         <v>3550308071</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73">
         <v>3550308072</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74">
         <v>3550308073</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74" s="2">
+        <v>10</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75">
         <v>3550308074</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76">
         <v>3550308075</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76" s="2">
+        <v>13</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77">
         <v>3550308076</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78">
         <v>3550308077</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79">
         <v>3550308078</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80">
         <v>3550308079</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81">
         <v>3550308080</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82">
         <v>3550308081</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>83</v>
       </c>
       <c r="B83">
         <v>3550308082</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84">
         <v>3550308083</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>85</v>
       </c>
       <c r="B85">
         <v>3550308084</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>86</v>
       </c>
       <c r="B86">
         <v>3550308085</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>87</v>
       </c>
       <c r="B87">
         <v>3550308086</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>88</v>
       </c>
       <c r="B88">
         <v>3550308087</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>89</v>
       </c>
       <c r="B89">
         <v>3550308088</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>90</v>
       </c>
       <c r="B90">
         <v>3550308089</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>91</v>
       </c>
       <c r="B91">
         <v>3550308090</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>92</v>
       </c>
       <c r="B92">
         <v>3550308091</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>97</v>
       </c>
       <c r="B93">
         <v>3550308092</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>93</v>
       </c>
       <c r="B94">
         <v>3550308093</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>94</v>
       </c>
       <c r="B95">
         <v>3550308094</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>95</v>
       </c>
       <c r="B96">
         <v>3550308095</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>96</v>
       </c>
       <c r="B97">
         <v>3550308096</v>
       </c>
+      <c r="C97" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>230</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D97" xr:uid="{567F9104-819A-6C4A-B2B3-7BA5B21804E4}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>